<commit_message>
made new planning and started class diagram
</commit_message>
<xml_diff>
--- a/Documentation/Agenda.xlsx
+++ b/Documentation/Agenda.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\PoolSideFM-Clone\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github\PoolSideFM-Clone\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C474BE3-E4AF-45F9-92A1-4D152F4D2CF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6D9030-C499-4305-9782-0F8C9E87623B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E7C21A0E-5B01-4304-BBBD-E8CB2CBC060E}"/>
+    <workbookView xWindow="3945" yWindow="4845" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{E7C21A0E-5B01-4304-BBBD-E8CB2CBC060E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="39">
   <si>
     <t>Analyse Document</t>
   </si>
@@ -130,6 +131,24 @@
   </si>
   <si>
     <t>Algoritmiek</t>
+  </si>
+  <si>
+    <t>leerdoel</t>
+  </si>
+  <si>
+    <t>in de vorm van</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Ontwerp document</t>
+  </si>
+  <si>
+    <t>Opnieuw schrijven wat ik gemaakt heb</t>
+  </si>
+  <si>
+    <t>Notities</t>
   </si>
 </sst>
 </file>
@@ -187,7 +206,157 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.749961851863155"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.749961851863155"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.749961851863155"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -550,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B269CD2-0D1A-49D4-89FD-9CACFEFB5CBA}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,6 +1043,190 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:H5 E5 E2 C2:D9 C10:E11 C23:D23 C13:D21">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+      <formula>"Ready for Review"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+      <formula>"Op pauze"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+      <formula>"Af"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
+      <formula>"Bezig"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+      <formula>"Niet begonnen"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{381898AD-E1D3-4116-9C9A-D96AB4405FE3}">
+  <dimension ref="A1:L19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="55.28515625" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="L1:L5">
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+      <formula>"Ready for Review"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+      <formula>"Op pauze"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+      <formula>"Af"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+      <formula>"Bezig"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+      <formula>"Niet begonnen"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C19 D2">
     <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"Ready for Review"</formula>
     </cfRule>

</xml_diff>